<commit_message>
fixed example and removed output from tracking
</commit_message>
<xml_diff>
--- a/example/data/Output/files/files_infos.xlsx
+++ b/example/data/Output/files/files_infos.xlsx
@@ -555,7 +555,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>CalDB</t>
+          <t>calibration</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -624,7 +624,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>CalDB</t>
+          <t>calibration</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -693,7 +693,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>CalDBder</t>
+          <t>deriv_calibration</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -762,7 +762,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>CalDBder</t>
+          <t>deriv_calibration</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -831,7 +831,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>CalDB</t>
+          <t>calibration</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -900,7 +900,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>CalDB</t>
+          <t>calibration</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">

</xml_diff>